<commit_message>
start big parser and fix problem with big class
</commit_message>
<xml_diff>
--- a/sorting/src/test/resources/BigClass.xlsx
+++ b/sorting/src/test/resources/BigClass.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arutf\Documents\classOrganization\sorting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE12A98-F0F3-46E1-B5EA-DAECC2BBB816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC6DEBC-F3E1-45E6-A7F3-9FD9165A9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -225,7 +225,7 @@
     <t>Forty,Fifty</t>
   </si>
   <si>
-    <t>One,Three</t>
+    <t>Eight,Five</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E532457-8704-43CC-9CC0-0F6573E68FA0}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F58" sqref="F58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
refactor tests and add big parser
</commit_message>
<xml_diff>
--- a/sorting/src/test/resources/BigClass.xlsx
+++ b/sorting/src/test/resources/BigClass.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arutf\Documents\classOrganization\sorting\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC6DEBC-F3E1-45E6-A7F3-9FD9165A9882}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406DFEAF-768E-4206-B3B5-B1489A835038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
+    <workbookView xWindow="38290" yWindow="-110" windowWidth="25820" windowHeight="18820" xr2:uid="{75A70F23-6CEA-406E-B64B-2FD3293A5F8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,13 +219,13 @@
     <t>Fifty</t>
   </si>
   <si>
-    <t>Fity-one</t>
-  </si>
-  <si>
     <t>Forty,Fifty</t>
   </si>
   <si>
     <t>Eight,Five</t>
+  </si>
+  <si>
+    <t>Fifty-one</t>
   </si>
 </sst>
 </file>
@@ -583,11 +583,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E532457-8704-43CC-9CC0-0F6573E68FA0}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="F58" sqref="F58"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="11.89453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
@@ -719,7 +722,7 @@
         <v>17</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G16" t="s">
         <v>25</v>
@@ -1062,12 +1065,12 @@
         <v>24</v>
       </c>
       <c r="F57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D58" t="s">
         <v>28</v>

</xml_diff>